<commit_message>
updating de data model draft with keys and updating the queries and datas of the 4 tables
</commit_message>
<xml_diff>
--- a/002-Ali AdventureWorks/Business Request & Planning/KPI's and DB Model.xlsx
+++ b/002-Ali AdventureWorks/Business Request & Planning/KPI's and DB Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Data Eng Roadmap\Projects\Data_Analysis\002-Ali AdventureWorks\Business Request &amp; Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AF634-C13E-4B55-B5ED-577E50F0BF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0663AB-290C-4349-8E21-5CF7FFA53A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="0" windowWidth="10968" windowHeight="12336" activeTab="1" xr2:uid="{CC38ABA3-B97F-4144-92A5-A0A757A64AC0}"/>
+    <workbookView xWindow="2904" yWindow="348" windowWidth="14076" windowHeight="11112" activeTab="1" xr2:uid="{CC38ABA3-B97F-4144-92A5-A0A757A64AC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrices" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>DIMENSIONS TABLES</t>
   </si>
@@ -89,6 +89,123 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>ProductKey</t>
+  </si>
+  <si>
+    <t>OrderDateKey</t>
+  </si>
+  <si>
+    <t>CustomerKey</t>
+  </si>
+  <si>
+    <t>CurrencyKey</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Order_Nbr</t>
+  </si>
+  <si>
+    <t>OrderQuantity</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>SalesAmount</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>DateKey</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>WeekNbr</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>MonthShort</t>
+  </si>
+  <si>
+    <t>MonthNbr</t>
+  </si>
+  <si>
+    <t>CalendarQuarter</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Full_Name</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>DateFirstPurchase</t>
+  </si>
+  <si>
+    <t>ProductItemCode</t>
+  </si>
+  <si>
+    <t>Prod_SubCategory</t>
+  </si>
+  <si>
+    <t>Prod_Category</t>
+  </si>
+  <si>
+    <t>Product_Name</t>
+  </si>
+  <si>
+    <t>StandardCost</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>SafetyStockLevel</t>
+  </si>
+  <si>
+    <t>SizeRange</t>
+  </si>
+  <si>
+    <t>ModelName</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>Prod_Status</t>
   </si>
 </sst>
 </file>
@@ -154,7 +271,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +293,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -270,6 +399,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -290,16 +431,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -516,20 +654,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F914948-3F2D-453D-AE26-F935778F371A}" name="Tableau1" displayName="Tableau1" ref="A3:K39" totalsRowShown="0" headerRowDxfId="12" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F914948-3F2D-453D-AE26-F935778F371A}" name="Tableau1" displayName="Tableau1" ref="A3:K39" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A3:K39" xr:uid="{43778763-EB19-4FD5-9F1E-49F483FD926C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{39382351-B70D-44DB-8F66-34A2852D267D}" name="FACTS TABLES" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{AB168EC8-AF10-4C4C-8BC3-79F390E3BCA4}" name="DIM_Calendar" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{572989F1-1EFF-4F1A-B3D3-3353DAFEBD9A}" name="DIM_Customers" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{85F1F85B-157B-4588-9DE0-99334F73D5E7}" name="DIM_Products" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{8E88E5AB-F5D2-4D92-9B5F-38F26CA8CA8A}" name=" 3" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{A4FA1503-B723-4550-BEE2-E94004C31131}" name=" 5" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{C4F52FD6-375B-4500-86FD-C51CA11EC5DD}" name=" 6" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{62F8D1A7-7228-4405-BD99-963E21EC602F}" name="6" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{20FEF3FD-AE53-491F-A37A-D5578E862954}" name=" 8" dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{77515E3D-DBEC-4F3B-808F-1D3379F5F96E}" name=" 7" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{ED44446B-3606-44E8-88CC-50D5581B3D8E}" name=" 9" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{39382351-B70D-44DB-8F66-34A2852D267D}" name="FACTS TABLES" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{AB168EC8-AF10-4C4C-8BC3-79F390E3BCA4}" name="DIM_Calendar" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{572989F1-1EFF-4F1A-B3D3-3353DAFEBD9A}" name="DIM_Customers" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{85F1F85B-157B-4588-9DE0-99334F73D5E7}" name="DIM_Products" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{8E88E5AB-F5D2-4D92-9B5F-38F26CA8CA8A}" name=" 3" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{A4FA1503-B723-4550-BEE2-E94004C31131}" name=" 5" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{C4F52FD6-375B-4500-86FD-C51CA11EC5DD}" name=" 6" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{62F8D1A7-7228-4405-BD99-963E21EC602F}" name="6" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{20FEF3FD-AE53-491F-A37A-D5578E862954}" name=" 8" dataDxfId="2"/>
+    <tableColumn id="28" xr3:uid="{77515E3D-DBEC-4F3B-808F-1D3379F5F96E}" name=" 7" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{ED44446B-3606-44E8-88CC-50D5581B3D8E}" name=" 9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -848,35 +986,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -918,480 +1056,480 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1411,50 +1549,51 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="4" customWidth="1"/>
-    <col min="2" max="6" width="15.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="4" customWidth="1"/>
+    <col min="3" max="6" width="15.5546875" style="4" customWidth="1"/>
     <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="str">
+      <c r="A3" s="12" t="str">
         <f>+Tableau1[[#Headers],[DIM_Calendar]]</f>
         <v>DIM_Calendar</v>
       </c>
-      <c r="B3" s="18" t="str">
+      <c r="B3" s="12" t="str">
         <f>+Tableau1[[#Headers],[DIM_Customers]]</f>
         <v>DIM_Customers</v>
       </c>
-      <c r="C3" s="18" t="str">
+      <c r="C3" s="12" t="str">
         <f>+Tableau1[[#Headers],[DIM_Products]]</f>
         <v>DIM_Products</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1467,262 +1606,345 @@
       <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="A4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="A5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="A6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="A7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="A8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="A10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="A12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="str">
+      <c r="A17" s="13" t="str">
         <f>+'Bus Matrices'!A4</f>
         <v>FACT_InternetSales</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="A18" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="A19" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="A20" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="A21" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
+      <c r="A22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="A23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
+      <c r="A24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="A25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="A26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
+      <c r="A27" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
+      <c r="A28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>

</xml_diff>